<commit_message>
changes for all scripts
</commit_message>
<xml_diff>
--- a/DM/databank/banking/deal_management/BANK_82_6_Test_43706.xlsx
+++ b/DM/databank/banking/deal_management/BANK_82_6_Test_43706.xlsx
@@ -12,7 +12,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="825" uniqueCount="440">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="460">
   <si>
     <t>SQ. NO.</t>
   </si>
@@ -1407,6 +1407,66 @@
   </si>
   <si>
     <t>213035745140</t>
+  </si>
+  <si>
+    <t>213658330808</t>
+  </si>
+  <si>
+    <t>213815924549</t>
+  </si>
+  <si>
+    <t>213581308843</t>
+  </si>
+  <si>
+    <t>213264425011</t>
+  </si>
+  <si>
+    <t>213651344640</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>213986856486</t>
+  </si>
+  <si>
+    <t>213337781580</t>
+  </si>
+  <si>
+    <t>213409451481</t>
+  </si>
+  <si>
+    <t>213286665082</t>
+  </si>
+  <si>
+    <t>213333396416</t>
+  </si>
+  <si>
+    <t>213181994210</t>
+  </si>
+  <si>
+    <t>213033302344</t>
+  </si>
+  <si>
+    <t>213790347424</t>
+  </si>
+  <si>
+    <t>213386817958</t>
+  </si>
+  <si>
+    <t>213570305187</t>
   </si>
 </sst>
 </file>
@@ -1776,7 +1836,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="125">
+  <cellXfs count="131">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -2011,6 +2071,78 @@
     <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="49" fontId="5" fillId="10" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="10" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="10" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="10" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2020,21 +2152,6 @@
     <xf numFmtId="0" fontId="11" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -2074,63 +2191,6 @@
     <xf numFmtId="0" fontId="11" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="10" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="10" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="10" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="10" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2140,6 +2200,18 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2423,13 +2495,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:DN132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H55" zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
-      <selection activeCell="O76" sqref="O76"/>
+    <sheetView tabSelected="1" topLeftCell="D124" zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
+      <selection activeCell="K133" sqref="K133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="16" width="24.6328125" customWidth="1" collapsed="1"/>
+    <col min="1" max="16" customWidth="true" width="24.6328125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:118" s="14" customFormat="1" ht="23.5" x14ac:dyDescent="0.35">
@@ -3161,11 +3233,11 @@
       <c r="I16" s="14"/>
     </row>
     <row r="18" spans="1:117" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="106" t="s">
+      <c r="A18" s="103" t="s">
         <v>178</v>
       </c>
-      <c r="B18" s="106"/>
-      <c r="C18" s="106"/>
+      <c r="B18" s="103"/>
+      <c r="C18" s="103"/>
     </row>
     <row r="19" spans="1:117" ht="62" x14ac:dyDescent="0.35">
       <c r="A19" s="26" t="s">
@@ -3215,24 +3287,24 @@
       <c r="E21" s="34"/>
     </row>
     <row r="23" spans="1:117" s="14" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="107" t="s">
+      <c r="A23" s="104" t="s">
         <v>186</v>
       </c>
-      <c r="B23" s="108"/>
-      <c r="C23" s="108"/>
-      <c r="D23" s="108"/>
-      <c r="E23" s="108"/>
-      <c r="F23" s="108"/>
-      <c r="G23" s="108"/>
-      <c r="H23" s="108"/>
-      <c r="I23" s="108"/>
-      <c r="J23" s="108"/>
-      <c r="K23" s="108"/>
-      <c r="L23" s="108"/>
-      <c r="M23" s="108"/>
-      <c r="N23" s="108"/>
-      <c r="O23" s="108"/>
-      <c r="P23" s="108"/>
+      <c r="B23" s="105"/>
+      <c r="C23" s="105"/>
+      <c r="D23" s="105"/>
+      <c r="E23" s="105"/>
+      <c r="F23" s="105"/>
+      <c r="G23" s="105"/>
+      <c r="H23" s="105"/>
+      <c r="I23" s="105"/>
+      <c r="J23" s="105"/>
+      <c r="K23" s="105"/>
+      <c r="L23" s="105"/>
+      <c r="M23" s="105"/>
+      <c r="N23" s="105"/>
+      <c r="O23" s="105"/>
+      <c r="P23" s="105"/>
       <c r="BM23" s="16"/>
       <c r="BN23" s="16"/>
       <c r="BO23" s="16"/>
@@ -6109,12 +6181,12 @@
       <c r="DM56" s="16"/>
     </row>
     <row r="58" spans="1:117" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="A58" s="109" t="s">
+      <c r="A58" s="82" t="s">
         <v>266</v>
       </c>
-      <c r="B58" s="110"/>
-      <c r="C58" s="110"/>
-      <c r="D58" s="111"/>
+      <c r="B58" s="83"/>
+      <c r="C58" s="83"/>
+      <c r="D58" s="84"/>
     </row>
     <row r="59" spans="1:117" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A59" s="26" t="s">
@@ -6150,12 +6222,12 @@
       </c>
     </row>
     <row r="62" spans="1:117" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="A62" s="109" t="s">
+      <c r="A62" s="82" t="s">
         <v>258</v>
       </c>
-      <c r="B62" s="110"/>
-      <c r="C62" s="110"/>
-      <c r="D62" s="111"/>
+      <c r="B62" s="83"/>
+      <c r="C62" s="83"/>
+      <c r="D62" s="84"/>
     </row>
     <row r="63" spans="1:117" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A63" s="26" t="s">
@@ -6242,17 +6314,17 @@
       <c r="G66" s="31"/>
     </row>
     <row r="68" spans="1:15" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="A68" s="109" t="s">
+      <c r="A68" s="82" t="s">
         <v>243</v>
       </c>
-      <c r="B68" s="110"/>
-      <c r="C68" s="110"/>
-      <c r="D68" s="110"/>
-      <c r="E68" s="110"/>
-      <c r="F68" s="110"/>
-      <c r="G68" s="110"/>
-      <c r="H68" s="110"/>
-      <c r="I68" s="111"/>
+      <c r="B68" s="83"/>
+      <c r="C68" s="83"/>
+      <c r="D68" s="83"/>
+      <c r="E68" s="83"/>
+      <c r="F68" s="83"/>
+      <c r="G68" s="83"/>
+      <c r="H68" s="83"/>
+      <c r="I68" s="84"/>
     </row>
     <row r="69" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A69" s="25" t="s">
@@ -6325,11 +6397,11 @@
       <c r="I70" s="31"/>
       <c r="J70" s="42" t="str">
         <f ca="1">TEXT(TODAY()-320,"DD-MMM-YY")</f>
-        <v>22-Sep-22</v>
+        <v>24-Sep-22</v>
       </c>
       <c r="K70" s="42" t="str">
         <f ca="1">TEXT(TODAY()-290,"DD-MMM-YY")</f>
-        <v>22-Oct-22</v>
+        <v>24-Oct-22</v>
       </c>
       <c r="L70" s="32" t="s">
         <v>174</v>
@@ -6368,11 +6440,11 @@
       <c r="I71" s="31"/>
       <c r="J71" s="42" t="str">
         <f ca="1">TEXT(TODAY()-289,"DD-MMM-YY")</f>
-        <v>23-Oct-22</v>
+        <v>25-Oct-22</v>
       </c>
       <c r="K71" s="42" t="str">
         <f ca="1">TEXT(TODAY()-259,"DD-MMM-YY")</f>
-        <v>22-Nov-22</v>
+        <v>24-Nov-22</v>
       </c>
       <c r="L71" s="32" t="s">
         <v>174</v>
@@ -6411,11 +6483,11 @@
       <c r="I72" s="31"/>
       <c r="J72" s="42" t="str">
         <f ca="1">TEXT(TODAY()-258,"DD-MMM-YY")</f>
-        <v>23-Nov-22</v>
+        <v>25-Nov-22</v>
       </c>
       <c r="K72" s="42" t="str">
         <f ca="1">TEXT(TODAY()-229,"DD-MMM-YY")</f>
-        <v>22-Dec-22</v>
+        <v>24-Dec-22</v>
       </c>
       <c r="L72" s="32" t="s">
         <v>174</v>
@@ -6462,11 +6534,11 @@
       </c>
       <c r="J73" s="42" t="str">
         <f ca="1">TEXT(TODAY()-381,"DD-MMM-YY")</f>
-        <v>23-Jul-22</v>
+        <v>25-Jul-22</v>
       </c>
       <c r="K73" s="42" t="str">
         <f ca="1">TEXT(TODAY()-351,"DD-MMM-YY")</f>
-        <v>22-Aug-22</v>
+        <v>24-Aug-22</v>
       </c>
       <c r="L73" s="32" t="s">
         <v>174</v>
@@ -6513,11 +6585,11 @@
       </c>
       <c r="J74" s="42" t="str">
         <f ca="1">TEXT(TODAY()-350,"DD-MMM-YY")</f>
-        <v>23-Aug-22</v>
+        <v>25-Aug-22</v>
       </c>
       <c r="K74" s="42" t="str">
         <f ca="1">TEXT(TODAY()-321,"DD-MMM-YY")</f>
-        <v>21-Sep-22</v>
+        <v>23-Sep-22</v>
       </c>
       <c r="L74" s="32" t="s">
         <v>174</v>
@@ -6533,27 +6605,27 @@
       </c>
     </row>
     <row r="76" spans="1:15" ht="50.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A76" s="115" t="s">
+      <c r="A76" s="88" t="s">
         <v>275</v>
       </c>
-      <c r="B76" s="115"/>
-      <c r="C76" s="115"/>
-      <c r="D76" s="115"/>
-      <c r="E76" s="115"/>
-      <c r="F76" s="115"/>
-      <c r="G76" s="115"/>
-      <c r="H76" s="115"/>
-      <c r="I76" s="115"/>
-      <c r="J76" s="115"/>
-      <c r="K76" s="115"/>
+      <c r="B76" s="88"/>
+      <c r="C76" s="88"/>
+      <c r="D76" s="88"/>
+      <c r="E76" s="88"/>
+      <c r="F76" s="88"/>
+      <c r="G76" s="88"/>
+      <c r="H76" s="88"/>
+      <c r="I76" s="88"/>
+      <c r="J76" s="88"/>
+      <c r="K76" s="88"/>
     </row>
     <row r="78" spans="1:15" ht="16.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A78" s="116" t="s">
+      <c r="A78" s="89" t="s">
         <v>276</v>
       </c>
-      <c r="B78" s="116"/>
-      <c r="C78" s="116"/>
-      <c r="D78" s="116"/>
+      <c r="B78" s="89"/>
+      <c r="C78" s="89"/>
+      <c r="D78" s="89"/>
     </row>
     <row r="79" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A79" s="43" t="s">
@@ -6680,33 +6752,33 @@
       <c r="S83" s="48" t="s">
         <v>301</v>
       </c>
-      <c r="T83" s="117" t="s">
+      <c r="T83" s="90" t="s">
         <v>302</v>
       </c>
-      <c r="U83" s="118"/>
-      <c r="V83" s="119"/>
-      <c r="W83" s="117" t="s">
+      <c r="U83" s="91"/>
+      <c r="V83" s="92"/>
+      <c r="W83" s="90" t="s">
         <v>303</v>
       </c>
-      <c r="X83" s="119"/>
+      <c r="X83" s="92"/>
       <c r="Y83" s="49"/>
-      <c r="Z83" s="112" t="s">
+      <c r="Z83" s="85" t="s">
         <v>304</v>
       </c>
-      <c r="AA83" s="113"/>
-      <c r="AB83" s="113"/>
-      <c r="AC83" s="113"/>
-      <c r="AD83" s="113"/>
-      <c r="AE83" s="113"/>
-      <c r="AF83" s="114"/>
-      <c r="AG83" s="112" t="s">
+      <c r="AA83" s="86"/>
+      <c r="AB83" s="86"/>
+      <c r="AC83" s="86"/>
+      <c r="AD83" s="86"/>
+      <c r="AE83" s="86"/>
+      <c r="AF83" s="87"/>
+      <c r="AG83" s="85" t="s">
         <v>305</v>
       </c>
-      <c r="AH83" s="113"/>
-      <c r="AI83" s="113"/>
-      <c r="AJ83" s="113"/>
-      <c r="AK83" s="113"/>
-      <c r="AL83" s="114"/>
+      <c r="AH83" s="86"/>
+      <c r="AI83" s="86"/>
+      <c r="AJ83" s="86"/>
+      <c r="AK83" s="86"/>
+      <c r="AL83" s="87"/>
       <c r="AM83" s="50"/>
       <c r="AN83" s="51"/>
       <c r="AO83" s="51"/>
@@ -6891,11 +6963,11 @@
       </c>
       <c r="G85" s="58" t="str">
         <f ca="1">TEXT(TODAY(),"YYYY-MM-DD")</f>
-        <v>2023-08-08</v>
+        <v>2023-08-10</v>
       </c>
       <c r="H85" s="58" t="str">
         <f ca="1">TEXT(TODAY(),"YYYY-MM-DD")</f>
-        <v>2023-08-08</v>
+        <v>2023-08-10</v>
       </c>
       <c r="I85" s="56">
         <v>12</v>
@@ -7138,7 +7210,7 @@
       </c>
       <c r="C89" s="34" t="str">
         <f ca="1">TEXT(TODAY(),"YYYY-MM-DD")</f>
-        <v>2023-08-08</v>
+        <v>2023-08-10</v>
       </c>
       <c r="D89" s="34" t="s">
         <v>157</v>
@@ -7148,7 +7220,7 @@
       </c>
       <c r="F89" s="62" t="str">
         <f ca="1">TEXT(TODAY(),"YYYY-MM-DD")</f>
-        <v>2023-08-08</v>
+        <v>2023-08-10</v>
       </c>
       <c r="G89" s="58" t="s">
         <v>332</v>
@@ -7200,7 +7272,7 @@
       </c>
       <c r="C90" s="34" t="str">
         <f ca="1">TEXT(TODAY(),"YYYY-MM-DD")</f>
-        <v>2023-08-08</v>
+        <v>2023-08-10</v>
       </c>
       <c r="D90" s="34" t="s">
         <v>157</v>
@@ -7210,7 +7282,7 @@
       </c>
       <c r="F90" s="62" t="str">
         <f ca="1">TEXT(TODAY(),"YYYY-MM-DD")</f>
-        <v>2023-08-08</v>
+        <v>2023-08-10</v>
       </c>
       <c r="G90" s="58" t="s">
         <v>332</v>
@@ -7254,63 +7326,63 @@
       <c r="BZ90" s="52"/>
     </row>
     <row r="92" spans="1:78" x14ac:dyDescent="0.35">
-      <c r="A92" s="103" t="s">
+      <c r="A92" s="100" t="s">
         <v>351</v>
       </c>
-      <c r="B92" s="104"/>
-      <c r="C92" s="104"/>
-      <c r="D92" s="104"/>
-      <c r="E92" s="104"/>
-      <c r="F92" s="104"/>
-      <c r="G92" s="104"/>
-      <c r="H92" s="104"/>
-      <c r="I92" s="104"/>
-      <c r="J92" s="104"/>
+      <c r="B92" s="101"/>
+      <c r="C92" s="101"/>
+      <c r="D92" s="101"/>
+      <c r="E92" s="101"/>
+      <c r="F92" s="101"/>
+      <c r="G92" s="101"/>
+      <c r="H92" s="101"/>
+      <c r="I92" s="101"/>
+      <c r="J92" s="101"/>
     </row>
     <row r="93" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A93" s="63"/>
       <c r="B93" s="64"/>
-      <c r="C93" s="105" t="s">
+      <c r="C93" s="102" t="s">
         <v>352</v>
       </c>
-      <c r="D93" s="105"/>
-      <c r="E93" s="105"/>
-      <c r="F93" s="105"/>
-      <c r="G93" s="105"/>
-      <c r="H93" s="105"/>
-      <c r="I93" s="105"/>
-      <c r="J93" s="105"/>
-      <c r="K93" s="105"/>
+      <c r="D93" s="102"/>
+      <c r="E93" s="102"/>
+      <c r="F93" s="102"/>
+      <c r="G93" s="102"/>
+      <c r="H93" s="102"/>
+      <c r="I93" s="102"/>
+      <c r="J93" s="102"/>
+      <c r="K93" s="102"/>
     </row>
     <row r="94" spans="1:78" x14ac:dyDescent="0.35">
-      <c r="A94" s="88" t="s">
+      <c r="A94" s="93" t="s">
         <v>353</v>
       </c>
-      <c r="B94" s="88" t="s">
+      <c r="B94" s="93" t="s">
         <v>354</v>
       </c>
-      <c r="C94" s="82" t="s">
+      <c r="C94" s="106" t="s">
         <v>355</v>
       </c>
-      <c r="D94" s="83"/>
-      <c r="E94" s="83"/>
-      <c r="F94" s="84"/>
-      <c r="G94" s="85" t="s">
+      <c r="D94" s="107"/>
+      <c r="E94" s="107"/>
+      <c r="F94" s="108"/>
+      <c r="G94" s="95" t="s">
         <v>356</v>
       </c>
-      <c r="H94" s="86"/>
-      <c r="I94" s="86"/>
-      <c r="J94" s="87"/>
-      <c r="K94" s="88" t="s">
+      <c r="H94" s="96"/>
+      <c r="I94" s="96"/>
+      <c r="J94" s="97"/>
+      <c r="K94" s="93" t="s">
         <v>357</v>
       </c>
-      <c r="L94" s="88" t="s">
+      <c r="L94" s="93" t="s">
         <v>358</v>
       </c>
     </row>
     <row r="95" spans="1:78" x14ac:dyDescent="0.35">
-      <c r="A95" s="89"/>
-      <c r="B95" s="89"/>
+      <c r="A95" s="94"/>
+      <c r="B95" s="94"/>
       <c r="C95" s="65" t="s">
         <v>359</v>
       </c>
@@ -7335,8 +7407,8 @@
       <c r="J95" s="66" t="s">
         <v>362</v>
       </c>
-      <c r="K95" s="89"/>
-      <c r="L95" s="89"/>
+      <c r="K95" s="94"/>
+      <c r="L95" s="94"/>
     </row>
     <row r="96" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A96" s="41" t="s">
@@ -7386,76 +7458,76 @@
       </c>
     </row>
     <row r="98" spans="1:26" ht="13.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A98" s="103" t="s">
+      <c r="A98" s="100" t="s">
         <v>365</v>
       </c>
-      <c r="B98" s="104"/>
-      <c r="C98" s="104"/>
-      <c r="D98" s="104"/>
-      <c r="E98" s="104"/>
-      <c r="F98" s="104"/>
-      <c r="G98" s="104"/>
-      <c r="H98" s="104"/>
-      <c r="I98" s="104"/>
-      <c r="J98" s="104"/>
-      <c r="K98" s="104"/>
-      <c r="L98" s="104"/>
+      <c r="B98" s="101"/>
+      <c r="C98" s="101"/>
+      <c r="D98" s="101"/>
+      <c r="E98" s="101"/>
+      <c r="F98" s="101"/>
+      <c r="G98" s="101"/>
+      <c r="H98" s="101"/>
+      <c r="I98" s="101"/>
+      <c r="J98" s="101"/>
+      <c r="K98" s="101"/>
+      <c r="L98" s="101"/>
     </row>
     <row r="99" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A99" s="93" t="s">
+      <c r="A99" s="112" t="s">
         <v>131</v>
       </c>
-      <c r="B99" s="93" t="s">
+      <c r="B99" s="112" t="s">
         <v>366</v>
       </c>
-      <c r="C99" s="96" t="s">
+      <c r="C99" s="115" t="s">
         <v>367</v>
       </c>
-      <c r="D99" s="99" t="s">
+      <c r="D99" s="118" t="s">
         <v>368</v>
       </c>
-      <c r="E99" s="102" t="s">
+      <c r="E99" s="121" t="s">
         <v>352</v>
       </c>
-      <c r="F99" s="102"/>
-      <c r="G99" s="102"/>
-      <c r="H99" s="102"/>
-      <c r="I99" s="92" t="s">
+      <c r="F99" s="121"/>
+      <c r="G99" s="121"/>
+      <c r="H99" s="121"/>
+      <c r="I99" s="111" t="s">
         <v>369</v>
       </c>
-      <c r="J99" s="92"/>
-      <c r="K99" s="92"/>
-      <c r="L99" s="92"/>
+      <c r="J99" s="111"/>
+      <c r="K99" s="111"/>
+      <c r="L99" s="111"/>
     </row>
     <row r="100" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A100" s="94"/>
-      <c r="B100" s="94"/>
-      <c r="C100" s="97"/>
-      <c r="D100" s="100"/>
-      <c r="E100" s="82" t="s">
+      <c r="A100" s="113"/>
+      <c r="B100" s="113"/>
+      <c r="C100" s="116"/>
+      <c r="D100" s="119"/>
+      <c r="E100" s="106" t="s">
         <v>370</v>
       </c>
-      <c r="F100" s="84"/>
-      <c r="G100" s="85" t="s">
+      <c r="F100" s="108"/>
+      <c r="G100" s="95" t="s">
         <v>356</v>
       </c>
-      <c r="H100" s="87"/>
-      <c r="I100" s="82" t="s">
+      <c r="H100" s="97"/>
+      <c r="I100" s="106" t="s">
         <v>370</v>
       </c>
-      <c r="J100" s="84"/>
-      <c r="K100" s="85" t="s">
+      <c r="J100" s="108"/>
+      <c r="K100" s="95" t="s">
         <v>356</v>
       </c>
-      <c r="L100" s="87"/>
+      <c r="L100" s="97"/>
     </row>
     <row r="101" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A101" s="95"/>
-      <c r="B101" s="95" t="s">
+      <c r="A101" s="114"/>
+      <c r="B101" s="114" t="s">
         <v>130</v>
       </c>
-      <c r="C101" s="98"/>
-      <c r="D101" s="101"/>
+      <c r="C101" s="117"/>
+      <c r="D101" s="120"/>
       <c r="E101" s="65" t="s">
         <v>371</v>
       </c>
@@ -7624,61 +7696,61 @@
       </c>
     </row>
     <row r="106" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A106" s="103" t="s">
+      <c r="A106" s="100" t="s">
         <v>376</v>
       </c>
-      <c r="B106" s="104"/>
-      <c r="C106" s="104"/>
-      <c r="D106" s="104"/>
-      <c r="E106" s="104"/>
-      <c r="F106" s="104"/>
-      <c r="G106" s="104"/>
-      <c r="H106" s="104"/>
-      <c r="I106" s="104"/>
-      <c r="J106" s="104"/>
+      <c r="B106" s="101"/>
+      <c r="C106" s="101"/>
+      <c r="D106" s="101"/>
+      <c r="E106" s="101"/>
+      <c r="F106" s="101"/>
+      <c r="G106" s="101"/>
+      <c r="H106" s="101"/>
+      <c r="I106" s="101"/>
+      <c r="J106" s="101"/>
     </row>
     <row r="107" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A107" s="63"/>
       <c r="B107" s="64"/>
-      <c r="C107" s="105" t="s">
+      <c r="C107" s="102" t="s">
         <v>352</v>
       </c>
-      <c r="D107" s="105"/>
-      <c r="E107" s="105"/>
-      <c r="F107" s="105"/>
-      <c r="G107" s="105"/>
-      <c r="H107" s="105"/>
-      <c r="I107" s="105"/>
-      <c r="J107" s="105"/>
-      <c r="K107" s="105"/>
+      <c r="D107" s="102"/>
+      <c r="E107" s="102"/>
+      <c r="F107" s="102"/>
+      <c r="G107" s="102"/>
+      <c r="H107" s="102"/>
+      <c r="I107" s="102"/>
+      <c r="J107" s="102"/>
+      <c r="K107" s="102"/>
       <c r="Z107" s="70"/>
     </row>
     <row r="108" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A108" s="88" t="s">
+      <c r="A108" s="93" t="s">
         <v>353</v>
       </c>
-      <c r="B108" s="88" t="s">
+      <c r="B108" s="93" t="s">
         <v>354</v>
       </c>
-      <c r="C108" s="82" t="s">
+      <c r="C108" s="106" t="s">
         <v>355</v>
       </c>
-      <c r="D108" s="83"/>
-      <c r="E108" s="83"/>
-      <c r="F108" s="84"/>
-      <c r="G108" s="85" t="s">
+      <c r="D108" s="107"/>
+      <c r="E108" s="107"/>
+      <c r="F108" s="108"/>
+      <c r="G108" s="95" t="s">
         <v>356</v>
       </c>
-      <c r="H108" s="86"/>
-      <c r="I108" s="86"/>
-      <c r="J108" s="87"/>
-      <c r="K108" s="120" t="s">
+      <c r="H108" s="96"/>
+      <c r="I108" s="96"/>
+      <c r="J108" s="97"/>
+      <c r="K108" s="98" t="s">
         <v>377</v>
       </c>
     </row>
     <row r="109" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A109" s="89"/>
-      <c r="B109" s="89"/>
+      <c r="A109" s="94"/>
+      <c r="B109" s="94"/>
       <c r="C109" s="65" t="s">
         <v>359</v>
       </c>
@@ -7703,7 +7775,7 @@
       <c r="J109" s="66" t="s">
         <v>362</v>
       </c>
-      <c r="K109" s="121"/>
+      <c r="K109" s="99"/>
     </row>
     <row r="110" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A110" s="56" t="s">
@@ -7814,7 +7886,7 @@
       <c r="I114" s="73"/>
       <c r="J114" s="74">
         <f ca="1">TODAY()</f>
-        <v>45146</v>
+        <v>45148</v>
       </c>
       <c r="K114" s="74">
         <v>234</v>
@@ -7847,7 +7919,7 @@
     <row r="118" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A118" s="75" t="str">
         <f ca="1">TEXT(TODAY(),"YYYY-MM-DD")</f>
-        <v>2023-08-08</v>
+        <v>2023-08-10</v>
       </c>
       <c r="B118" s="76" t="s">
         <v>396</v>
@@ -7862,7 +7934,7 @@
     <row r="119" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A119" s="75" t="str">
         <f ca="1">TEXT(TODAY(),"YYYY-MM-DD")</f>
-        <v>2023-08-08</v>
+        <v>2023-08-10</v>
       </c>
       <c r="B119" s="76" t="s">
         <v>398</v>
@@ -7877,7 +7949,7 @@
     <row r="120" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A120" s="75" t="str">
         <f ca="1">TEXT(TODAY(),"YYYY-MM-DD")</f>
-        <v>2023-08-08</v>
+        <v>2023-08-10</v>
       </c>
       <c r="B120" s="76" t="s">
         <v>397</v>
@@ -7890,26 +7962,26 @@
       </c>
     </row>
     <row r="122" spans="1:47" x14ac:dyDescent="0.35">
-      <c r="A122" s="90" t="s">
+      <c r="A122" s="109" t="s">
         <v>423</v>
       </c>
-      <c r="B122" s="91"/>
-      <c r="C122" s="91"/>
-      <c r="D122" s="91"/>
-      <c r="E122" s="91"/>
-      <c r="F122" s="91"/>
-      <c r="G122" s="91"/>
-      <c r="H122" s="91"/>
-      <c r="I122" s="91"/>
-      <c r="J122" s="91"/>
-      <c r="K122" s="91"/>
-      <c r="L122" s="91"/>
-      <c r="M122" s="91"/>
-      <c r="N122" s="91"/>
-      <c r="O122" s="91"/>
-      <c r="P122" s="91"/>
-      <c r="Q122" s="91"/>
-      <c r="R122" s="91"/>
+      <c r="B122" s="110"/>
+      <c r="C122" s="110"/>
+      <c r="D122" s="110"/>
+      <c r="E122" s="110"/>
+      <c r="F122" s="110"/>
+      <c r="G122" s="110"/>
+      <c r="H122" s="110"/>
+      <c r="I122" s="110"/>
+      <c r="J122" s="110"/>
+      <c r="K122" s="110"/>
+      <c r="L122" s="110"/>
+      <c r="M122" s="110"/>
+      <c r="N122" s="110"/>
+      <c r="O122" s="110"/>
+      <c r="P122" s="110"/>
+      <c r="Q122" s="110"/>
+      <c r="R122" s="110"/>
       <c r="S122" s="64"/>
       <c r="T122" s="64"/>
       <c r="U122" s="64"/>
@@ -8009,7 +8081,7 @@
       </c>
       <c r="D124" s="80" t="str">
         <f ca="1">TEXT(TODAY(),"YYYY-MM-DD")</f>
-        <v>2023-08-08</v>
+        <v>2023-08-10</v>
       </c>
       <c r="E124" s="80"/>
       <c r="F124" s="81">
@@ -8067,17 +8139,17 @@
       </c>
     </row>
     <row r="126" spans="1:47" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="A126" s="109" t="s">
+      <c r="A126" s="82" t="s">
         <v>243</v>
       </c>
-      <c r="B126" s="110"/>
-      <c r="C126" s="110"/>
-      <c r="D126" s="110"/>
-      <c r="E126" s="110"/>
-      <c r="F126" s="110"/>
-      <c r="G126" s="110"/>
-      <c r="H126" s="110"/>
-      <c r="I126" s="111"/>
+      <c r="B126" s="83"/>
+      <c r="C126" s="83"/>
+      <c r="D126" s="83"/>
+      <c r="E126" s="83"/>
+      <c r="F126" s="83"/>
+      <c r="G126" s="83"/>
+      <c r="H126" s="83"/>
+      <c r="I126" s="84"/>
     </row>
     <row r="127" spans="1:47" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A127" s="25" t="s">
@@ -8127,231 +8199,231 @@
       </c>
     </row>
     <row r="128" spans="1:47" x14ac:dyDescent="0.35">
-      <c r="A128" s="28" t="s">
+      <c r="A128" s="126" t="s">
         <v>428</v>
       </c>
-      <c r="B128" s="28" t="str">
+      <c r="B128" s="40" t="str">
         <f>C10</f>
         <v>2131846854</v>
       </c>
-      <c r="C128" s="28" t="s">
+      <c r="C128" s="40" t="s">
         <v>430</v>
       </c>
       <c r="D128" s="30" t="str">
         <f>C16</f>
         <v>2131846279</v>
       </c>
-      <c r="E128" s="31" t="s">
+      <c r="E128" s="127" t="s">
         <v>177</v>
       </c>
-      <c r="F128" s="31"/>
-      <c r="G128" s="31"/>
-      <c r="H128" s="31"/>
-      <c r="I128" s="31"/>
-      <c r="J128" s="42" t="str">
+      <c r="F128" s="125"/>
+      <c r="G128" s="125"/>
+      <c r="H128" s="125"/>
+      <c r="I128" s="125"/>
+      <c r="J128" s="129" t="str">
         <f ca="1">TEXT(TODAY()-320,"MM-DD-YYYY")</f>
-        <v>09-22-2022</v>
-      </c>
-      <c r="K128" s="42" t="str">
+        <v>09-24-2022</v>
+      </c>
+      <c r="K128" s="129" t="str">
         <f ca="1">TEXT(TODAY()-290,"MM-DD-YYYY")</f>
-        <v>10-22-2022</v>
+        <v>10-24-2022</v>
       </c>
       <c r="L128" s="32" t="s">
         <v>174</v>
       </c>
-      <c r="M128" s="32">
-        <v>12</v>
+      <c r="M128" s="128" t="s">
+        <v>445</v>
       </c>
       <c r="N128" s="44" t="s">
-        <v>435</v>
+        <v>455</v>
       </c>
       <c r="O128" s="32" t="s">
         <v>349</v>
       </c>
     </row>
     <row r="129" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A129" s="28" t="s">
+      <c r="A129" s="126" t="s">
         <v>428</v>
       </c>
-      <c r="B129" s="28" t="str">
+      <c r="B129" s="40" t="str">
         <f>C10</f>
         <v>2131846854</v>
       </c>
-      <c r="C129" s="28" t="s">
+      <c r="C129" s="40" t="s">
         <v>430</v>
       </c>
       <c r="D129" s="30" t="str">
         <f>C16</f>
         <v>2131846279</v>
       </c>
-      <c r="E129" s="31" t="s">
+      <c r="E129" s="127" t="s">
         <v>177</v>
       </c>
-      <c r="F129" s="31"/>
-      <c r="G129" s="31"/>
-      <c r="H129" s="31"/>
-      <c r="I129" s="31"/>
-      <c r="J129" s="42" t="str">
+      <c r="F129" s="125"/>
+      <c r="G129" s="125"/>
+      <c r="H129" s="125"/>
+      <c r="I129" s="125"/>
+      <c r="J129" s="129" t="str">
         <f ca="1">TEXT(TODAY()-289,"MM-DD-YYYY")</f>
-        <v>10-23-2022</v>
-      </c>
-      <c r="K129" s="42" t="str">
+        <v>10-25-2022</v>
+      </c>
+      <c r="K129" s="129" t="str">
         <f ca="1">TEXT(TODAY()-259,"MM-DD-YYYY")</f>
-        <v>11-22-2022</v>
+        <v>11-24-2022</v>
       </c>
       <c r="L129" s="32" t="s">
         <v>174</v>
       </c>
-      <c r="M129" s="32">
-        <v>13</v>
+      <c r="M129" s="128" t="s">
+        <v>446</v>
       </c>
       <c r="N129" s="44" t="s">
-        <v>436</v>
+        <v>456</v>
       </c>
       <c r="O129" s="32" t="s">
         <v>349</v>
       </c>
     </row>
     <row r="130" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A130" s="28" t="s">
+      <c r="A130" s="126" t="s">
         <v>428</v>
       </c>
-      <c r="B130" s="28" t="str">
+      <c r="B130" s="40" t="str">
         <f>C10</f>
         <v>2131846854</v>
       </c>
-      <c r="C130" s="28" t="s">
+      <c r="C130" s="40" t="s">
         <v>430</v>
       </c>
       <c r="D130" s="30" t="str">
         <f>C16</f>
         <v>2131846279</v>
       </c>
-      <c r="E130" s="31" t="s">
+      <c r="E130" s="127" t="s">
         <v>254</v>
       </c>
-      <c r="F130" s="31"/>
-      <c r="G130" s="31"/>
-      <c r="H130" s="31"/>
-      <c r="I130" s="31"/>
-      <c r="J130" s="42" t="str">
+      <c r="F130" s="125"/>
+      <c r="G130" s="125"/>
+      <c r="H130" s="125"/>
+      <c r="I130" s="125"/>
+      <c r="J130" s="129" t="str">
         <f ca="1">TEXT(TODAY()-258,"MM-DD-YYYY")</f>
-        <v>11-23-2022</v>
-      </c>
-      <c r="K130" s="42" t="str">
+        <v>11-25-2022</v>
+      </c>
+      <c r="K130" s="129" t="str">
         <f ca="1">TEXT(TODAY()-229,"MM-DD-YYYY")</f>
-        <v>12-22-2022</v>
+        <v>12-24-2022</v>
       </c>
       <c r="L130" s="32" t="s">
         <v>174</v>
       </c>
-      <c r="M130" s="32">
-        <v>6</v>
+      <c r="M130" s="128" t="s">
+        <v>447</v>
       </c>
       <c r="N130" s="44" t="s">
-        <v>437</v>
+        <v>457</v>
       </c>
       <c r="O130" s="32" t="s">
         <v>349</v>
       </c>
     </row>
     <row r="131" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A131" s="28" t="s">
+      <c r="A131" s="126" t="s">
         <v>428</v>
       </c>
-      <c r="B131" s="28" t="str">
+      <c r="B131" s="40" t="str">
         <f>C10</f>
         <v>2131846854</v>
       </c>
-      <c r="C131" s="28" t="s">
+      <c r="C131" s="40" t="s">
         <v>430</v>
       </c>
       <c r="D131" s="30" t="str">
         <f>C16</f>
         <v>2131846279</v>
       </c>
-      <c r="E131" s="31" t="s">
+      <c r="E131" s="127" t="s">
         <v>253</v>
       </c>
-      <c r="F131" s="31" t="s">
+      <c r="F131" s="127" t="s">
         <v>267</v>
       </c>
-      <c r="G131" s="31" t="s">
+      <c r="G131" s="127" t="s">
         <v>157</v>
       </c>
-      <c r="H131" s="31" t="s">
+      <c r="H131" s="127" t="s">
         <v>268</v>
       </c>
-      <c r="I131" s="31" t="s">
+      <c r="I131" s="127" t="s">
         <v>269</v>
       </c>
-      <c r="J131" s="42" t="str">
+      <c r="J131" s="129" t="str">
         <f ca="1">TEXT(TODAY()-381,"MM-DD-YYYY")</f>
-        <v>07-23-2022</v>
-      </c>
-      <c r="K131" s="42" t="str">
+        <v>07-25-2022</v>
+      </c>
+      <c r="K131" s="129" t="str">
         <f ca="1">TEXT(TODAY()-351,"MM-DD-YYYY")</f>
-        <v>08-22-2022</v>
+        <v>08-24-2022</v>
       </c>
       <c r="L131" s="32" t="s">
         <v>174</v>
       </c>
-      <c r="M131" s="32">
-        <v>7</v>
+      <c r="M131" s="128" t="s">
+        <v>448</v>
       </c>
       <c r="N131" s="44" t="s">
-        <v>438</v>
+        <v>458</v>
       </c>
       <c r="O131" s="32" t="s">
         <v>349</v>
       </c>
     </row>
     <row r="132" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A132" s="28" t="s">
+      <c r="A132" s="126" t="s">
         <v>428</v>
       </c>
-      <c r="B132" s="41" t="str">
+      <c r="B132" s="30" t="str">
         <f>C10</f>
         <v>2131846854</v>
       </c>
-      <c r="C132" s="28" t="s">
+      <c r="C132" s="40" t="s">
         <v>430</v>
       </c>
       <c r="D132" s="30" t="str">
         <f>C16</f>
         <v>2131846279</v>
       </c>
-      <c r="E132" s="31" t="s">
+      <c r="E132" s="127" t="s">
         <v>253</v>
       </c>
-      <c r="F132" s="31" t="s">
+      <c r="F132" s="127" t="s">
         <v>267</v>
       </c>
-      <c r="G132" s="31" t="s">
+      <c r="G132" s="127" t="s">
         <v>157</v>
       </c>
-      <c r="H132" s="31" t="s">
+      <c r="H132" s="127" t="s">
         <v>268</v>
       </c>
-      <c r="I132" s="31" t="s">
+      <c r="I132" s="127" t="s">
         <v>274</v>
       </c>
-      <c r="J132" s="42" t="str">
+      <c r="J132" s="129" t="str">
         <f ca="1">TEXT(TODAY()-350,"MM-DD-YYYY")</f>
-        <v>08-23-2022</v>
-      </c>
-      <c r="K132" s="42" t="str">
+        <v>08-25-2022</v>
+      </c>
+      <c r="K132" s="130" t="str">
         <f ca="1">TEXT(TODAY()-321,"MM-DD-YYYY")</f>
-        <v>09-21-2022</v>
+        <v>09-23-2022</v>
       </c>
       <c r="L132" s="32" t="s">
         <v>174</v>
       </c>
-      <c r="M132" s="32">
-        <v>10</v>
+      <c r="M132" s="128" t="s">
+        <v>449</v>
       </c>
       <c r="N132" s="44" t="s">
-        <v>439</v>
+        <v>459</v>
       </c>
       <c r="O132" s="32" t="s">
         <v>349</v>
@@ -8359,6 +8431,29 @@
     </row>
   </sheetData>
   <mergeCells count="39">
+    <mergeCell ref="A122:R122"/>
+    <mergeCell ref="I99:L99"/>
+    <mergeCell ref="E100:F100"/>
+    <mergeCell ref="G100:H100"/>
+    <mergeCell ref="I100:J100"/>
+    <mergeCell ref="K100:L100"/>
+    <mergeCell ref="A99:A101"/>
+    <mergeCell ref="B99:B101"/>
+    <mergeCell ref="C99:C101"/>
+    <mergeCell ref="D99:D101"/>
+    <mergeCell ref="E99:H99"/>
+    <mergeCell ref="A106:J106"/>
+    <mergeCell ref="C107:K107"/>
+    <mergeCell ref="A108:A109"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A23:P23"/>
+    <mergeCell ref="A68:I68"/>
+    <mergeCell ref="A62:D62"/>
+    <mergeCell ref="A58:D58"/>
+    <mergeCell ref="C94:F94"/>
+    <mergeCell ref="G94:J94"/>
+    <mergeCell ref="C108:F108"/>
+    <mergeCell ref="K94:K95"/>
     <mergeCell ref="A126:I126"/>
     <mergeCell ref="AG83:AL83"/>
     <mergeCell ref="A76:K76"/>
@@ -8375,29 +8470,6 @@
     <mergeCell ref="C93:K93"/>
     <mergeCell ref="A94:A95"/>
     <mergeCell ref="B94:B95"/>
-    <mergeCell ref="C107:K107"/>
-    <mergeCell ref="A108:A109"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="A23:P23"/>
-    <mergeCell ref="A68:I68"/>
-    <mergeCell ref="A62:D62"/>
-    <mergeCell ref="A58:D58"/>
-    <mergeCell ref="C94:F94"/>
-    <mergeCell ref="G94:J94"/>
-    <mergeCell ref="C108:F108"/>
-    <mergeCell ref="K94:K95"/>
-    <mergeCell ref="A122:R122"/>
-    <mergeCell ref="I99:L99"/>
-    <mergeCell ref="E100:F100"/>
-    <mergeCell ref="G100:H100"/>
-    <mergeCell ref="I100:J100"/>
-    <mergeCell ref="K100:L100"/>
-    <mergeCell ref="A99:A101"/>
-    <mergeCell ref="B99:B101"/>
-    <mergeCell ref="C99:C101"/>
-    <mergeCell ref="D99:D101"/>
-    <mergeCell ref="E99:H99"/>
-    <mergeCell ref="A106:J106"/>
   </mergeCells>
   <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C14 C58 MZJ124 NJF124 NTB124 OCX124 OMT124 OWP124 PGL124 PQH124 QAD124 QJZ124 QTV124 RDR124 RNN124 RXJ124 SHF124 SRB124 TAX124 TKT124 TUP124 UEL124 UOH124 UYD124 VHZ124 VRV124 WBR124 WLN124 WVJ124 IX124 ST124 ACP124 AML124 AWH124 BGD124 BPZ124 BZV124 CJR124 CTN124 DDJ124 DNF124 DXB124 EGX124 EQT124 FAP124 LCD124 FKL124 FUH124 GED124 GNZ124 GXV124 HHR124 HRN124 IBJ124 ILF124 IVB124 JEX124 JOT124 JYP124 KIL124 KSH124 LLZ124 LVV124 MFR124 MPN124">
@@ -8429,13 +8501,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="13" max="13" width="21.453125" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="13.26953125" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="36.90625" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="42" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="44.90625" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="59.26953125" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="22.54296875" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" customWidth="true" width="21.453125" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="13.26953125" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="36.90625" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="42.0" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="44.90625" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" width="59.26953125" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" width="22.54296875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="52" x14ac:dyDescent="0.35">

</xml_diff>